<commit_message>
Modification du fichier InfoJOueur.xlsx
</commit_message>
<xml_diff>
--- a/Fichiers/InfoJoueur.xlsx
+++ b/Fichiers/InfoJoueur.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Dortmund" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,10 @@
     <sheet name="Real_Madrid" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Manchester_United" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="PSG" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Feuille13" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Bayern" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Naple" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Tottenham" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Milan" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="715">
   <si>
     <t xml:space="preserve">Prenom</t>
   </si>
@@ -1931,6 +1934,252 @@
   </si>
   <si>
     <t xml:space="preserve">Müller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luigii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sepe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hrvoje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chirichs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roumanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elseid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hysaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalidou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koulibaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faouzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghoulam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albiol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorenzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jorginho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamsik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovaquie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piotr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zieliński</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zinédine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amadou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diawara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Callejon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mertens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leandrinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insigne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ounas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkadiuz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hugo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lloris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tottenham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gazzaniga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kieran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trippier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alderweireld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertoghen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foyth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkers-Peters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanyama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sissokho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erikson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heug-min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coree-du-Sud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moura</t>
   </si>
 </sst>
 </file>
@@ -2005,9 +2254,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2030,18 +2283,18 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.47448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.24489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2623,10 +2876,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3135,10 +3391,13 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="A1:F1 H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3719,14 +3978,12 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+      <selection pane="topLeft" activeCell="N26" activeCellId="1" sqref="A1:F1 N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5102040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,8 +4481,552 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5714285714286"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>605</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>617</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>628</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>631</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -4255,111 +5056,703 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>475</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>591</v>
+        <v>633</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>592</v>
+        <v>125</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>594</v>
+        <v>635</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>595</v>
+        <v>636</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>592</v>
+        <v>213</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>637</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>596</v>
+        <v>638</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>592</v>
+        <v>103</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>597</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>598</v>
+        <v>639</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>592</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>599</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>600</v>
+        <v>640</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>592</v>
+        <v>213</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>601</v>
+        <v>641</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>602</v>
+        <v>642</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>603</v>
+        <v>643</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>644</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>125</v>
+        <v>645</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>604</v>
+        <v>646</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>605</v>
+        <v>647</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>592</v>
+        <v>648</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>593</v>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>649</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>650</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>657</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4367,234 +5760,366 @@
         <v>418</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>606</v>
+        <v>693</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>103</v>
+        <v>184</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>607</v>
+        <v>694</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>608</v>
+        <v>695</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>592</v>
+        <v>369</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>609</v>
+        <v>135</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>610</v>
+        <v>696</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>611</v>
+        <v>87</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>44</v>
+        <v>697</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>612</v>
+        <v>698</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>611</v>
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>560</v>
+        <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>613</v>
+        <v>699</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>103</v>
+        <v>184</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>614</v>
+        <v>300</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>615</v>
+        <v>700</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>701</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>616</v>
+        <v>510</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>617</v>
+        <v>702</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>92</v>
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>618</v>
+        <v>703</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>244</v>
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>558</v>
+        <v>253</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>619</v>
+        <v>460</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>592</v>
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>620</v>
+        <v>704</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>439</v>
+        <v>705</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>335</v>
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>621</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>622</v>
+        <v>706</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>17</v>
+        <v>309</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>623</v>
+        <v>707</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>624</v>
+        <v>708</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>625</v>
+        <v>709</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>626</v>
+        <v>710</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>592</v>
+        <v>711</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>627</v>
+        <v>712</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>628</v>
+        <v>713</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>592</v>
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>359</v>
+        <v>284</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>629</v>
+        <v>487</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>592</v>
+        <v>103</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>593</v>
+        <v>681</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>630</v>
+        <v>182</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>631</v>
+        <v>714</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>31</v>
+        <v>125</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>632</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>592</v>
+        <v>681</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4616,17 +6141,17 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="1" sqref="A1:F1 C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.48469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5168,10 +6693,13 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5769,10 +7297,13 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6421,10 +7952,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6833,10 +8367,13 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7325,10 +8862,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7843,10 +9383,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8367,10 +9910,13 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>